<commit_message>
Update to Kongasis land value error April 11, 2021
</commit_message>
<xml_diff>
--- a/InvestmentRiskDashboard.xlsx
+++ b/InvestmentRiskDashboard.xlsx
@@ -651,7 +651,7 @@
       <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -675,7 +675,7 @@
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2492,10 +2492,10 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.91"/>
@@ -2595,7 +2595,7 @@
         <v>4000000</v>
       </c>
       <c r="G3" s="9" t="n">
-        <v>50000</v>
+        <v>5000000</v>
       </c>
       <c r="H3" s="7" t="n">
         <v>20000</v>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="J3" s="9" t="n">
         <f aca="false">G3*I3</f>
-        <v>50000</v>
+        <v>5000000</v>
       </c>
       <c r="K3" s="5"/>
     </row>

</xml_diff>